<commit_message>
Correccion 05 - Finalize OK hasta Cordova
</commit_message>
<xml_diff>
--- a/correcion 05.xlsx
+++ b/correcion 05.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esome\AppData\Development\Boot_80973\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{22FD6D0F-71C1-4830-87D8-63C80AC2095F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE34B73-2145-468C-AE66-C4261AD257C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{CD148A91-9792-45E8-A487-7C936E81F5CE}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="8">
   <si>
     <t>ok</t>
   </si>
@@ -52,6 +52,15 @@
   </si>
   <si>
     <t xml:space="preserve">ok </t>
+  </si>
+  <si>
+    <t>cohecha</t>
+  </si>
+  <si>
+    <t>ok-</t>
+  </si>
+  <si>
+    <t>Cordova</t>
   </si>
 </sst>
 </file>
@@ -412,7 +421,7 @@
   <dimension ref="B3:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,8 +437,12 @@
       <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
@@ -442,8 +455,12 @@
       <c r="D4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
@@ -456,8 +473,12 @@
       <c r="D5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -470,8 +491,12 @@
       <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
@@ -484,8 +509,12 @@
       <c r="D7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
@@ -498,8 +527,12 @@
       <c r="D8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -512,8 +545,12 @@
       <c r="D9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -526,8 +563,12 @@
       <c r="D10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
@@ -540,8 +581,12 @@
       <c r="D11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -554,8 +599,12 @@
       <c r="D12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
@@ -568,8 +617,12 @@
       <c r="D13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
@@ -582,8 +635,12 @@
       <c r="D14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
@@ -596,8 +653,12 @@
       <c r="D15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G15" s="2"/>
     </row>
   </sheetData>

</xml_diff>